<commit_message>
fix: update excel and seeder
</commit_message>
<xml_diff>
--- a/perhitungan case base reasoning.XLSX
+++ b/perhitungan case base reasoning.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jodyk\OneDrive\Documents\Projects\laravel\project\exsys-cf-gkm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BF1D8E-81AF-40C3-BC7B-4D4D3F9023B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CF4E28-3ADD-48AA-A836-75EF2298BF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -290,9 +290,6 @@
     <t xml:space="preserve">Tabel Sistem Pakar </t>
   </si>
   <si>
-    <t>Gangguan Meis Kronis</t>
-  </si>
-  <si>
     <t>Gangguan Penggunaan Zat</t>
   </si>
   <si>
@@ -338,9 +335,6 @@
     <t>total bbt dari gjl yg sama</t>
   </si>
   <si>
-    <t>Hasil diagniosa adalah Depresi dengan hasil =</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -351,6 +345,12 @@
   </si>
   <si>
     <t>Hitung hasil</t>
+  </si>
+  <si>
+    <t>Gangguan Medis Kronis</t>
+  </si>
+  <si>
+    <t>Hasil diagniosa adalah Somatoform dengan hasil =</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -851,12 +851,78 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -875,15 +941,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -908,782 +967,41 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="108">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2282,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Z104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="E34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,30 +1636,30 @@
       </c>
     </row>
     <row r="2" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
@@ -2351,19 +1669,16 @@
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="12"/>
-      <c r="F3" s="23"/>
       <c r="G3" s="10" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="13"/>
       <c r="I3" s="12"/>
-      <c r="J3" s="23"/>
       <c r="K3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="L3" s="13"/>
       <c r="M3" s="12"/>
-      <c r="N3" s="23"/>
       <c r="O3" s="10" t="s">
         <v>8</v>
       </c>
@@ -2371,7 +1686,6 @@
       <c r="Q3" s="13"/>
       <c r="R3" s="13"/>
       <c r="S3" s="12"/>
-      <c r="T3" s="23"/>
       <c r="U3" s="10" t="s">
         <v>11</v>
       </c>
@@ -2392,7 +1706,6 @@
       <c r="E4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="23"/>
       <c r="G4" s="10" t="s">
         <v>1</v>
       </c>
@@ -2402,7 +1715,6 @@
       <c r="I4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="23"/>
       <c r="K4" s="10" t="s">
         <v>1</v>
       </c>
@@ -2412,7 +1724,6 @@
       <c r="M4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="23"/>
       <c r="O4" s="10" t="s">
         <v>1</v>
       </c>
@@ -2428,7 +1739,6 @@
       <c r="S4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="T4" s="23"/>
       <c r="U4" s="10" t="s">
         <v>1</v>
       </c>
@@ -2457,7 +1767,6 @@
       <c r="E5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="23"/>
       <c r="G5" s="2">
         <v>1</v>
       </c>
@@ -2467,7 +1776,6 @@
       <c r="I5" s="3">
         <v>1</v>
       </c>
-      <c r="J5" s="23"/>
       <c r="K5" s="2">
         <v>1</v>
       </c>
@@ -2475,16 +1783,15 @@
         <v>84</v>
       </c>
       <c r="M5" s="3">
-        <v>5</v>
-      </c>
-      <c r="N5" s="23"/>
+        <v>3</v>
+      </c>
       <c r="O5" s="2">
         <v>1</v>
       </c>
       <c r="P5" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="Q5" s="23" t="s">
+      <c r="Q5" t="s">
         <v>62</v>
       </c>
       <c r="R5" s="8" t="s">
@@ -2493,14 +1800,13 @@
       <c r="S5" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="T5" s="23"/>
       <c r="U5" s="2">
         <v>1</v>
       </c>
       <c r="V5" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="W5" s="23" t="s">
+      <c r="W5" t="s">
         <v>72</v>
       </c>
       <c r="X5" s="8">
@@ -2522,7 +1828,6 @@
       <c r="E6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="23"/>
       <c r="G6" s="2">
         <v>2</v>
       </c>
@@ -2532,24 +1837,22 @@
       <c r="I6" s="3">
         <v>3</v>
       </c>
-      <c r="J6" s="23"/>
       <c r="K6" s="2">
         <v>2</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="M6" s="3">
-        <v>3</v>
-      </c>
-      <c r="N6" s="23"/>
+        <v>5</v>
+      </c>
       <c r="O6" s="2">
         <v>2</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="Q6" s="23" t="s">
+      <c r="Q6" t="s">
         <v>63</v>
       </c>
       <c r="R6" s="8" t="s">
@@ -2558,14 +1861,13 @@
       <c r="S6" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="T6" s="23"/>
       <c r="U6" s="2">
         <v>2</v>
       </c>
       <c r="V6" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="W6" s="23" t="s">
+      <c r="W6" t="s">
         <v>73</v>
       </c>
       <c r="X6" s="8">
@@ -2587,7 +1889,6 @@
       <c r="E7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="23"/>
       <c r="G7" s="4">
         <v>3</v>
       </c>
@@ -2597,24 +1898,22 @@
       <c r="I7" s="6">
         <v>5</v>
       </c>
-      <c r="J7" s="23"/>
       <c r="K7" s="2">
         <v>3</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M7" s="3">
         <v>5</v>
       </c>
-      <c r="N7" s="23"/>
       <c r="O7" s="2">
         <v>3</v>
       </c>
       <c r="P7" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="Q7" s="23" t="s">
+      <c r="Q7" t="s">
         <v>64</v>
       </c>
       <c r="R7" s="8" t="s">
@@ -2623,14 +1922,13 @@
       <c r="S7" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="T7" s="23"/>
       <c r="U7" s="2">
         <v>3</v>
       </c>
       <c r="V7" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="W7" s="23" t="s">
+      <c r="W7" t="s">
         <v>74</v>
       </c>
       <c r="X7" s="8">
@@ -2652,21 +1950,15 @@
       <c r="E8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="24">
+      <c r="K8" s="4">
         <v>4</v>
       </c>
-      <c r="L8" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="M8" s="25">
+      <c r="L8" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="M8" s="6">
         <v>3</v>
       </c>
-      <c r="N8" s="23"/>
       <c r="O8" s="4">
         <v>4</v>
       </c>
@@ -2682,7 +1974,6 @@
       <c r="S8" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="T8" s="23"/>
       <c r="U8" s="4">
         <v>4</v>
       </c>
@@ -2711,26 +2002,6 @@
       <c r="E9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="23"/>
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
@@ -2744,26 +2015,6 @@
       <c r="E10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
-      <c r="X10" s="23"/>
-      <c r="Y10" s="23"/>
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.25">
@@ -2777,26 +2028,6 @@
       <c r="E11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="23"/>
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.25">
@@ -2810,26 +2041,6 @@
       <c r="E12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="23"/>
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
@@ -2843,26 +2054,6 @@
       <c r="E13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="23"/>
-      <c r="X13" s="23"/>
-      <c r="Y13" s="23"/>
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.25">
@@ -2876,26 +2067,6 @@
       <c r="E14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="23"/>
-      <c r="X14" s="23"/>
-      <c r="Y14" s="23"/>
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.25">
@@ -2909,26 +2080,6 @@
       <c r="E15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="23"/>
-      <c r="X15" s="23"/>
-      <c r="Y15" s="23"/>
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.25">
@@ -2942,26 +2093,6 @@
       <c r="E16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="23"/>
-      <c r="Y16" s="23"/>
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="2:26" x14ac:dyDescent="0.25">
@@ -2975,26 +2106,6 @@
       <c r="E17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="23"/>
-      <c r="X17" s="23"/>
-      <c r="Y17" s="23"/>
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="2:26" x14ac:dyDescent="0.25">
@@ -3008,26 +2119,6 @@
       <c r="E18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="23"/>
-      <c r="V18" s="23"/>
-      <c r="W18" s="23"/>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="23"/>
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="2:26" x14ac:dyDescent="0.25">
@@ -3041,26 +2132,6 @@
       <c r="E19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="23"/>
-      <c r="V19" s="23"/>
-      <c r="W19" s="23"/>
-      <c r="X19" s="23"/>
-      <c r="Y19" s="23"/>
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="2:26" x14ac:dyDescent="0.25">
@@ -3074,26 +2145,6 @@
       <c r="E20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="23"/>
-      <c r="V20" s="23"/>
-      <c r="W20" s="23"/>
-      <c r="X20" s="23"/>
-      <c r="Y20" s="23"/>
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="2:26" x14ac:dyDescent="0.25">
@@ -3107,26 +2158,6 @@
       <c r="E21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
-      <c r="U21" s="23"/>
-      <c r="V21" s="23"/>
-      <c r="W21" s="23"/>
-      <c r="X21" s="23"/>
-      <c r="Y21" s="23"/>
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="2:26" x14ac:dyDescent="0.25">
@@ -3140,26 +2171,6 @@
       <c r="E22" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="23"/>
-      <c r="S22" s="23"/>
-      <c r="T22" s="23"/>
-      <c r="U22" s="23"/>
-      <c r="V22" s="23"/>
-      <c r="W22" s="23"/>
-      <c r="X22" s="23"/>
-      <c r="Y22" s="23"/>
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="2:26" x14ac:dyDescent="0.25">
@@ -3173,26 +2184,6 @@
       <c r="E23" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="23"/>
-      <c r="V23" s="23"/>
-      <c r="W23" s="23"/>
-      <c r="X23" s="23"/>
-      <c r="Y23" s="23"/>
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="2:26" x14ac:dyDescent="0.25">
@@ -3206,26 +2197,6 @@
       <c r="E24" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="23"/>
-      <c r="T24" s="23"/>
-      <c r="U24" s="23"/>
-      <c r="V24" s="23"/>
-      <c r="W24" s="23"/>
-      <c r="X24" s="23"/>
-      <c r="Y24" s="23"/>
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="2:26" x14ac:dyDescent="0.25">
@@ -3255,100 +2226,62 @@
       <c r="Y25" s="5"/>
       <c r="Z25" s="6"/>
     </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="23"/>
-      <c r="X26" s="23"/>
-      <c r="Y26" s="23"/>
-      <c r="Z26" s="23"/>
-    </row>
     <row r="27" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B27" s="21"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="22"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
       <c r="S27" s="1"/>
     </row>
     <row r="28" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
-      <c r="C28" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23" t="s">
+      <c r="C28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="20"/>
+      <c r="I28" t="s">
         <v>79</v>
       </c>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
       <c r="S28" s="3"/>
     </row>
     <row r="29" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
-      <c r="C29" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="23"/>
+      <c r="C29" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="38"/>
       <c r="I29" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
       <c r="L29" s="12"/>
       <c r="M29" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="N29" s="13"/>
       <c r="O29" s="12"/>
       <c r="P29" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q29" s="13"/>
       <c r="R29" s="12"/>
@@ -3356,22 +2289,21 @@
     </row>
     <row r="30" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="38" t="s">
+      <c r="E30" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="F30" s="30" t="s">
+      <c r="F30" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G30" s="44"/>
-      <c r="H30" s="23"/>
+      <c r="G30" s="37"/>
       <c r="I30" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J30" s="11" t="s">
         <v>77</v>
@@ -3382,49 +2314,48 @@
       <c r="L30" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="M30" s="51" t="s">
+      <c r="M30" s="7" t="s">
         <v>1</v>
       </c>
       <c r="N30" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="O30" s="11" t="s">
+      <c r="O30" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="P30" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="P30" s="55" t="s">
+      <c r="Q30" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="Q30" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="R30" s="55" t="s">
+      <c r="R30" s="11" t="s">
         <v>80</v>
       </c>
       <c r="S30" s="3"/>
     </row>
     <row r="31" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
-      <c r="C31" s="35">
+      <c r="C31" s="28">
         <v>1</v>
       </c>
-      <c r="D31" s="41" t="s">
+      <c r="D31" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="39" t="s">
+      <c r="E31" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="47">
+      <c r="F31" s="40">
         <v>2</v>
       </c>
-      <c r="G31" s="44"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="21">
+      <c r="G31" s="37"/>
+      <c r="I31" s="18">
         <v>1</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="K31" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="K31" s="19" t="s">
         <v>63</v>
       </c>
       <c r="L31" s="7" t="s">
@@ -3433,227 +2364,232 @@
       <c r="M31" s="7">
         <v>1</v>
       </c>
-      <c r="N31" s="7">
-        <v>5</v>
-      </c>
-      <c r="O31" s="7"/>
-      <c r="P31" s="21">
+      <c r="N31" s="18">
+        <v>5</v>
+      </c>
+      <c r="O31" s="7">
+        <f>IF(COUNTIF($F$31:$F$38,M31)=0,M31*0,M31*1)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="19">
         <f>SUM(N31:N37)</f>
         <v>31</v>
       </c>
       <c r="Q31" s="7">
         <f>SUM(O31:O37)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="R31" s="1">
         <f>Q31/P31</f>
-        <v>0.25806451612903225</v>
+        <v>0.16129032258064516</v>
       </c>
       <c r="S31" s="3"/>
     </row>
     <row r="32" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="40" t="s">
+      <c r="C32" s="29"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="48">
+      <c r="F32" s="41">
         <v>9</v>
       </c>
-      <c r="G32" s="45"/>
-      <c r="H32" s="23"/>
+      <c r="G32" s="38"/>
       <c r="I32" s="2"/>
       <c r="J32" s="8"/>
-      <c r="K32" s="23"/>
       <c r="L32" s="8" t="s">
         <v>37</v>
       </c>
       <c r="M32" s="8">
         <v>3</v>
       </c>
-      <c r="N32" s="8">
+      <c r="N32" s="2">
         <v>3</v>
       </c>
-      <c r="O32" s="8"/>
-      <c r="P32" s="2"/>
+      <c r="O32" s="8">
+        <f t="shared" ref="O32:O36" si="0">IF(COUNTIF($F$31:$F$38,M32)=0,M32*0,M32*1)</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="51"/>
       <c r="Q32" s="8"/>
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="40" t="s">
+      <c r="C33" s="29"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="F33" s="48">
+      <c r="F33" s="41">
         <v>10</v>
       </c>
-      <c r="G33" s="45"/>
-      <c r="H33" s="23"/>
+      <c r="G33" s="38"/>
       <c r="I33" s="2"/>
       <c r="J33" s="8"/>
-      <c r="K33" s="23"/>
       <c r="L33" s="8" t="s">
         <v>39</v>
       </c>
       <c r="M33" s="8">
         <v>5</v>
       </c>
-      <c r="N33" s="8">
-        <v>5</v>
-      </c>
-      <c r="O33" s="8"/>
-      <c r="P33" s="2"/>
+      <c r="N33" s="2">
+        <v>5</v>
+      </c>
+      <c r="O33" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P33" s="51"/>
       <c r="Q33" s="8"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="40" t="s">
+      <c r="C34" s="29"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="42">
+      <c r="F34" s="35">
         <v>14</v>
       </c>
-      <c r="G34" s="44"/>
-      <c r="H34" s="23"/>
+      <c r="G34" s="37"/>
       <c r="I34" s="2"/>
       <c r="J34" s="8"/>
-      <c r="K34" s="23"/>
       <c r="L34" s="8" t="s">
         <v>45</v>
       </c>
       <c r="M34" s="8">
         <v>11</v>
       </c>
-      <c r="N34" s="8">
-        <v>5</v>
-      </c>
-      <c r="O34" s="8"/>
-      <c r="P34" s="2"/>
+      <c r="N34" s="2">
+        <v>5</v>
+      </c>
+      <c r="O34" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P34" s="51"/>
       <c r="Q34" s="8"/>
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="42"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="35"/>
       <c r="E35" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F35" s="42">
+      <c r="F35" s="35">
         <v>16</v>
       </c>
-      <c r="G35" s="44"/>
-      <c r="H35" s="23"/>
+      <c r="G35" s="37"/>
       <c r="I35" s="2"/>
       <c r="J35" s="8"/>
-      <c r="K35" s="23"/>
       <c r="L35" s="8" t="s">
         <v>52</v>
       </c>
       <c r="M35" s="8">
         <v>18</v>
       </c>
-      <c r="N35" s="8">
-        <v>5</v>
-      </c>
-      <c r="O35" s="8"/>
-      <c r="P35" s="2"/>
+      <c r="N35" s="52">
+        <v>5</v>
+      </c>
+      <c r="O35" s="53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P35" s="51"/>
       <c r="Q35" s="8"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="52" t="s">
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="F36" s="48">
+      <c r="F36" s="41">
         <v>7</v>
       </c>
-      <c r="G36" s="45"/>
-      <c r="H36" s="23"/>
+      <c r="G36" s="38"/>
       <c r="I36" s="2"/>
       <c r="J36" s="8"/>
-      <c r="K36" s="23"/>
       <c r="L36" s="9" t="s">
         <v>54</v>
       </c>
       <c r="M36" s="9">
         <v>20</v>
       </c>
-      <c r="N36" s="19">
-        <v>5</v>
-      </c>
-      <c r="O36" s="19">
-        <v>5</v>
-      </c>
-      <c r="P36" s="2"/>
+      <c r="N36" s="54">
+        <v>5</v>
+      </c>
+      <c r="O36" s="55">
+        <f>IF(COUNTIF($F$31:$F$38,M36)=0,N36*0,N36*1)</f>
+        <v>5</v>
+      </c>
+      <c r="P36" s="51"/>
       <c r="Q36" s="8"/>
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="39" t="s">
+      <c r="C37" s="29"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="F37" s="42">
+      <c r="F37" s="35">
         <v>19</v>
       </c>
-      <c r="G37" s="44"/>
-      <c r="H37" s="23"/>
+      <c r="G37" s="37"/>
       <c r="I37" s="4"/>
       <c r="J37" s="9"/>
       <c r="K37" s="5"/>
       <c r="L37" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M37" s="9">
+        <v>1</v>
+      </c>
+      <c r="N37" s="56">
         <v>3</v>
       </c>
-      <c r="N37" s="19">
-        <v>3</v>
-      </c>
-      <c r="O37" s="19">
-        <v>3</v>
-      </c>
-      <c r="P37" s="2"/>
+      <c r="O37" s="57">
+        <f>IF(COUNTIF($F$39,M37)=0,N37*0,N37*1)</f>
+        <v>0</v>
+      </c>
+      <c r="P37" s="51"/>
       <c r="Q37" s="8"/>
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="43" t="s">
+      <c r="C38" s="29"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="43">
+      <c r="F38" s="36">
         <v>20</v>
       </c>
-      <c r="G38" s="44"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="21">
+      <c r="G38" s="37"/>
+      <c r="I38" s="18">
         <v>2</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K38" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="K38" s="19" t="s">
         <v>62</v>
       </c>
       <c r="L38" s="7" t="s">
@@ -3662,13 +2598,14 @@
       <c r="M38" s="8">
         <v>2</v>
       </c>
-      <c r="N38" s="20">
+      <c r="N38" s="58">
         <v>3</v>
       </c>
-      <c r="O38" s="20">
+      <c r="O38" s="59">
+        <f>IF(COUNTIF($F$31:$F$38,M38)=0,N38*0,N38*1)</f>
         <v>3</v>
       </c>
-      <c r="P38" s="21">
+      <c r="P38" s="19">
         <f>SUM(N38:N46)</f>
         <v>41</v>
       </c>
@@ -3677,247 +2614,247 @@
         <v>23</v>
       </c>
       <c r="R38" s="1">
-        <f t="shared" ref="R32:R56" si="0">Q38/P38</f>
+        <f t="shared" ref="R38:R52" si="1">Q38/P38</f>
         <v>0.56097560975609762</v>
       </c>
       <c r="S38" s="3"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="F39" s="54">
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F39" s="45">
         <v>3</v>
       </c>
-      <c r="G39" s="44"/>
-      <c r="H39" s="23"/>
+      <c r="G39" s="37"/>
       <c r="I39" s="2"/>
       <c r="J39" s="8"/>
-      <c r="K39" s="23"/>
       <c r="L39" s="8" t="s">
         <v>37</v>
       </c>
       <c r="M39" s="8">
         <v>3</v>
       </c>
-      <c r="N39" s="8">
+      <c r="N39" s="60">
         <v>3</v>
       </c>
-      <c r="O39" s="8"/>
-      <c r="P39" s="2"/>
+      <c r="O39" s="61">
+        <f t="shared" ref="O39:O45" si="2">IF(COUNTIF($F$31:$F$38,M39)=0,N39*0,N39*1)</f>
+        <v>0</v>
+      </c>
+      <c r="P39" s="51"/>
       <c r="Q39" s="8"/>
       <c r="R39" s="3"/>
       <c r="S39" s="3"/>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="23"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="37"/>
       <c r="I40" s="2"/>
       <c r="J40" s="8"/>
-      <c r="K40" s="23"/>
       <c r="L40" s="8" t="s">
         <v>43</v>
       </c>
       <c r="M40" s="8">
         <v>9</v>
       </c>
-      <c r="N40" s="18">
-        <v>5</v>
-      </c>
-      <c r="O40" s="18">
-        <v>5</v>
-      </c>
-      <c r="P40" s="2"/>
+      <c r="N40" s="62">
+        <v>5</v>
+      </c>
+      <c r="O40" s="55">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="P40" s="51"/>
       <c r="Q40" s="8"/>
       <c r="R40" s="3"/>
       <c r="S40" s="3"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="23"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="21"/>
       <c r="I41" s="2"/>
       <c r="J41" s="8"/>
-      <c r="K41" s="23"/>
       <c r="L41" s="8" t="s">
         <v>44</v>
       </c>
       <c r="M41" s="8">
         <v>10</v>
       </c>
-      <c r="N41" s="18">
-        <v>5</v>
-      </c>
-      <c r="O41" s="18">
-        <v>5</v>
-      </c>
-      <c r="P41" s="2"/>
+      <c r="N41" s="63">
+        <v>5</v>
+      </c>
+      <c r="O41" s="41">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="P41" s="51"/>
       <c r="Q41" s="8"/>
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="23"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
       <c r="I42" s="2"/>
       <c r="J42" s="8"/>
-      <c r="K42" s="23"/>
       <c r="L42" s="8" t="s">
         <v>45</v>
       </c>
       <c r="M42" s="8">
         <v>11</v>
       </c>
-      <c r="N42" s="8">
-        <v>5</v>
-      </c>
-      <c r="O42" s="8"/>
-      <c r="P42" s="2"/>
+      <c r="N42" s="64">
+        <v>5</v>
+      </c>
+      <c r="O42" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P42" s="51"/>
       <c r="Q42" s="8"/>
       <c r="R42" s="3"/>
       <c r="S42" s="3"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="2"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="72"/>
+      <c r="H43" s="3"/>
       <c r="J43" s="8"/>
-      <c r="K43" s="23"/>
       <c r="L43" s="8" t="s">
         <v>50</v>
       </c>
       <c r="M43" s="8">
         <v>16</v>
       </c>
-      <c r="N43" s="18">
-        <v>5</v>
-      </c>
-      <c r="O43" s="18">
-        <v>5</v>
-      </c>
-      <c r="P43" s="2"/>
+      <c r="N43" s="65">
+        <v>5</v>
+      </c>
+      <c r="O43" s="66">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="P43" s="51"/>
       <c r="Q43" s="8"/>
       <c r="R43" s="3"/>
       <c r="S43" s="3"/>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="23"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
       <c r="I44" s="2"/>
       <c r="J44" s="8"/>
-      <c r="K44" s="23"/>
       <c r="L44" s="8" t="s">
         <v>52</v>
       </c>
       <c r="M44" s="8">
         <v>18</v>
       </c>
-      <c r="N44" s="8">
-        <v>5</v>
-      </c>
-      <c r="O44" s="8"/>
-      <c r="P44" s="2"/>
+      <c r="N44" s="64">
+        <v>5</v>
+      </c>
+      <c r="O44" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P44" s="51"/>
       <c r="Q44" s="8"/>
       <c r="R44" s="3"/>
       <c r="S44" s="3"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="23"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
       <c r="I45" s="2"/>
       <c r="J45" s="8"/>
-      <c r="K45" s="23"/>
       <c r="L45" s="9" t="s">
         <v>54</v>
       </c>
       <c r="M45" s="9">
         <v>20</v>
       </c>
-      <c r="N45" s="19">
-        <v>5</v>
-      </c>
-      <c r="O45" s="19">
-        <v>5</v>
-      </c>
-      <c r="P45" s="2"/>
+      <c r="N45" s="56">
+        <v>5</v>
+      </c>
+      <c r="O45" s="59">
+        <f>IF(COUNTIF($F$31:$F$38,M45)=0,N45*0,N45*1)</f>
+        <v>5</v>
+      </c>
+      <c r="P45" s="51"/>
       <c r="Q45" s="8"/>
       <c r="R45" s="3"/>
       <c r="S45" s="3"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="23"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
       <c r="I46" s="4"/>
       <c r="J46" s="9"/>
       <c r="K46" s="5"/>
       <c r="L46" s="9" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="M46" s="8">
-        <v>5</v>
-      </c>
-      <c r="N46" s="9">
-        <v>5</v>
-      </c>
-      <c r="O46" s="9"/>
-      <c r="P46" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="N46" s="67">
+        <v>5</v>
+      </c>
+      <c r="O46" s="23">
+        <f>IF(COUNTIF($F$39,M46)=0,N46*0,N46*1)</f>
+        <v>0</v>
+      </c>
+      <c r="P46" s="5"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="6"/>
       <c r="S46" s="3"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="21">
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="I47" s="18">
         <v>3</v>
       </c>
       <c r="J47" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K47" s="19" t="s">
         <v>92</v>
-      </c>
-      <c r="K47" s="22" t="s">
-        <v>93</v>
       </c>
       <c r="L47" s="7" t="s">
         <v>35</v>
@@ -3925,148 +2862,151 @@
       <c r="M47" s="7">
         <v>1</v>
       </c>
-      <c r="N47" s="7">
-        <v>5</v>
-      </c>
-      <c r="O47" s="7"/>
-      <c r="P47" s="2">
+      <c r="N47" s="68">
+        <v>5</v>
+      </c>
+      <c r="O47" s="69">
+        <f>IF(COUNTIF($F$31:$F$38,M47)=0,N47*0,N47*1)</f>
+        <v>0</v>
+      </c>
+      <c r="P47" s="51">
         <f>SUM(N47:N51)</f>
         <v>21</v>
       </c>
       <c r="Q47" s="8">
         <f>SUM(O47:O51)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="R47" s="3">
-        <f t="shared" si="0"/>
-        <v>0.38095238095238093</v>
+        <f t="shared" si="1"/>
+        <v>0.61904761904761907</v>
       </c>
       <c r="S47" s="3"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="28"/>
-      <c r="G48" s="28"/>
-      <c r="H48" s="23"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
       <c r="I48" s="2"/>
       <c r="J48" s="8"/>
-      <c r="K48" s="23"/>
       <c r="L48" s="8" t="s">
         <v>37</v>
       </c>
       <c r="M48" s="8">
         <v>3</v>
       </c>
-      <c r="N48" s="8">
+      <c r="N48" s="70">
         <v>3</v>
       </c>
-      <c r="O48" s="8"/>
-      <c r="P48" s="2"/>
+      <c r="O48" s="35">
+        <f t="shared" ref="O48:O50" si="3">IF(COUNTIF($F$31:$F$38,M48)=0,N48*0,N48*1)</f>
+        <v>0</v>
+      </c>
+      <c r="P48" s="51"/>
       <c r="Q48" s="8"/>
       <c r="R48" s="3"/>
       <c r="S48" s="3"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="23"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
       <c r="I49" s="2"/>
       <c r="J49" s="8"/>
-      <c r="K49" s="23"/>
       <c r="L49" s="8" t="s">
         <v>41</v>
       </c>
       <c r="M49" s="8">
         <v>7</v>
       </c>
-      <c r="N49" s="18">
+      <c r="N49" s="65">
         <v>3</v>
       </c>
-      <c r="O49" s="18">
+      <c r="O49" s="66">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="P49" s="2"/>
+      <c r="P49" s="51"/>
       <c r="Q49" s="8"/>
       <c r="R49" s="3"/>
       <c r="S49" s="3"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="23"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
       <c r="I50" s="2"/>
       <c r="J50" s="8"/>
-      <c r="K50" s="23"/>
       <c r="L50" s="9" t="s">
         <v>53</v>
       </c>
       <c r="M50" s="9">
         <v>19</v>
       </c>
-      <c r="N50" s="19">
-        <v>5</v>
-      </c>
-      <c r="O50" s="19">
-        <v>5</v>
-      </c>
-      <c r="P50" s="2"/>
+      <c r="N50" s="56">
+        <v>5</v>
+      </c>
+      <c r="O50" s="59">
+        <f>IF(COUNTIF($F$31:$F$38,M50)=0,N50*0,N50*1)</f>
+        <v>5</v>
+      </c>
+      <c r="P50" s="51"/>
       <c r="Q50" s="8"/>
       <c r="R50" s="3"/>
       <c r="S50" s="3"/>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="28"/>
-      <c r="G51" s="28"/>
-      <c r="H51" s="23"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
       <c r="I51" s="4"/>
       <c r="J51" s="9"/>
       <c r="K51" s="5"/>
       <c r="L51" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M51" s="9">
-        <v>5</v>
-      </c>
-      <c r="N51" s="9">
-        <v>5</v>
-      </c>
-      <c r="O51" s="9"/>
-      <c r="P51" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="N51" s="27">
+        <v>5</v>
+      </c>
+      <c r="O51" s="23">
+        <f>IF(COUNTIF($F$39,M51)=0,N51*0,N51*1)</f>
+        <v>5</v>
+      </c>
+      <c r="P51" s="51"/>
       <c r="Q51" s="8"/>
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="28"/>
-      <c r="H52" s="23"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
       <c r="I52" s="2">
         <v>4</v>
       </c>
       <c r="J52" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="K52" t="s">
         <v>94</v>
-      </c>
-      <c r="K52" s="23" t="s">
-        <v>95</v>
       </c>
       <c r="L52" s="8" t="s">
         <v>37</v>
@@ -4074,186 +3014,171 @@
       <c r="M52" s="8">
         <v>3</v>
       </c>
-      <c r="N52" s="8">
-        <v>5</v>
-      </c>
-      <c r="O52" s="8"/>
-      <c r="P52" s="21">
+      <c r="N52" s="64">
+        <v>5</v>
+      </c>
+      <c r="O52" s="34">
+        <f>IF(COUNTIF($F$31:$F$38,M52)=0,N52*0,N52*1)</f>
+        <v>0</v>
+      </c>
+      <c r="P52" s="19">
         <f>SUM(N52:N56)</f>
         <v>23</v>
       </c>
       <c r="Q52" s="7">
         <f>SUM(O52:O56)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="R52" s="1">
-        <f t="shared" si="0"/>
-        <v>0.34782608695652173</v>
+        <f t="shared" si="1"/>
+        <v>0.21739130434782608</v>
       </c>
       <c r="S52" s="3"/>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="28"/>
-      <c r="H53" s="23"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
       <c r="I53" s="2"/>
       <c r="J53" s="8"/>
-      <c r="K53" s="23"/>
       <c r="L53" s="8" t="s">
         <v>42</v>
       </c>
       <c r="M53" s="8">
         <v>8</v>
       </c>
-      <c r="N53" s="8">
-        <v>5</v>
-      </c>
-      <c r="O53" s="8"/>
-      <c r="P53" s="2"/>
+      <c r="N53" s="64">
+        <v>5</v>
+      </c>
+      <c r="O53" s="34">
+        <f t="shared" ref="O53:O55" si="4">IF(COUNTIF($F$31:$F$38,M53)=0,N53*0,N53*1)</f>
+        <v>0</v>
+      </c>
+      <c r="P53" s="51"/>
       <c r="Q53" s="8"/>
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="28"/>
-      <c r="G54" s="28"/>
-      <c r="H54" s="23"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
       <c r="I54" s="2"/>
       <c r="J54" s="8"/>
-      <c r="K54" s="23"/>
       <c r="L54" s="8" t="s">
         <v>47</v>
       </c>
       <c r="M54" s="8">
         <v>13</v>
       </c>
-      <c r="N54" s="8">
-        <v>5</v>
-      </c>
-      <c r="O54" s="8"/>
-      <c r="P54" s="2"/>
+      <c r="N54" s="64">
+        <v>5</v>
+      </c>
+      <c r="O54" s="34">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P54" s="51"/>
       <c r="Q54" s="8"/>
       <c r="R54" s="3"/>
       <c r="S54" s="3"/>
     </row>
     <row r="55" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="23"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
       <c r="I55" s="2"/>
       <c r="J55" s="8"/>
-      <c r="K55" s="23"/>
       <c r="L55" s="9" t="s">
         <v>54</v>
       </c>
       <c r="M55" s="9">
         <v>20</v>
       </c>
-      <c r="N55" s="19">
-        <v>5</v>
-      </c>
-      <c r="O55" s="19">
-        <v>5</v>
-      </c>
-      <c r="P55" s="2"/>
+      <c r="N55" s="56">
+        <v>5</v>
+      </c>
+      <c r="O55" s="59">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="P55" s="51"/>
       <c r="Q55" s="8"/>
       <c r="R55" s="3"/>
       <c r="S55" s="3"/>
     </row>
     <row r="56" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B56" s="2"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="23"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
       <c r="I56" s="4"/>
       <c r="J56" s="9"/>
       <c r="K56" s="5"/>
-      <c r="L56" s="26" t="s">
-        <v>87</v>
+      <c r="L56" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="M56" s="9">
+        <v>4</v>
+      </c>
+      <c r="N56" s="71">
         <v>3</v>
       </c>
-      <c r="N56" s="19">
-        <v>3</v>
-      </c>
-      <c r="O56" s="19">
-        <v>3</v>
-      </c>
-      <c r="P56" s="4"/>
+      <c r="O56" s="57">
+        <f>IF(COUNTIF($F$39,M56)=0,N56*0,N56*1)</f>
+        <v>0</v>
+      </c>
+      <c r="P56" s="5"/>
       <c r="Q56" s="9"/>
       <c r="R56" s="6"/>
       <c r="S56" s="3"/>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="23"/>
-      <c r="I57" s="23"/>
-      <c r="J57" s="23"/>
-      <c r="K57" s="23"/>
-      <c r="L57" s="23"/>
-      <c r="M57" s="23"/>
-      <c r="N57" s="23"/>
-      <c r="O57" s="23"/>
-      <c r="P57" s="23"/>
-      <c r="Q57" s="23"/>
-      <c r="R57" s="23"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
       <c r="S57" s="3"/>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="27"/>
-      <c r="G58" s="27"/>
-      <c r="H58" s="23"/>
-      <c r="I58" s="23"/>
-      <c r="J58" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="K58" s="23"/>
-      <c r="L58" s="23">
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="J58" t="s">
+        <v>104</v>
+      </c>
+      <c r="L58">
         <f>MAX(R31:R56)</f>
-        <v>0.56097560975609762</v>
-      </c>
-      <c r="M58" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="N58" s="23"/>
-      <c r="O58" s="23"/>
-      <c r="P58" s="23"/>
-      <c r="Q58" s="23"/>
-      <c r="R58" s="23"/>
+        <v>0.61904761904761907</v>
+      </c>
+      <c r="M58" t="s">
+        <v>99</v>
+      </c>
       <c r="S58" s="3"/>
     </row>
     <row r="59" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B59" s="4"/>
-      <c r="C59" s="59"/>
-      <c r="D59" s="59"/>
-      <c r="E59" s="59"/>
-      <c r="F59" s="60"/>
-      <c r="G59" s="60"/>
+      <c r="C59" s="49"/>
+      <c r="D59" s="49"/>
+      <c r="E59" s="49"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="50"/>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
@@ -4268,425 +3193,406 @@
       <c r="S59" s="6"/>
     </row>
     <row r="60" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C60" s="32"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="46"/>
-      <c r="G60" s="46"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="39"/>
     </row>
     <row r="61" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C61" s="27"/>
-      <c r="D61" s="27"/>
-      <c r="E61" s="27"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="28"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="21"/>
     </row>
     <row r="63" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C63" s="49"/>
-      <c r="D63" s="49"/>
-      <c r="E63" s="49"/>
-      <c r="F63" s="49"/>
-      <c r="G63" s="49"/>
-      <c r="H63" s="49"/>
+      <c r="C63" s="42"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="42"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="42"/>
+      <c r="H63" s="42"/>
     </row>
     <row r="64" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C64" s="49"/>
-      <c r="D64" s="49"/>
-      <c r="E64" s="49"/>
-      <c r="F64" s="49"/>
-      <c r="G64" s="49"/>
-      <c r="H64" s="49"/>
-      <c r="M64" s="23"/>
-      <c r="N64" s="23"/>
-      <c r="O64" s="23"/>
-      <c r="P64" s="23"/>
-    </row>
-    <row r="65" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C65" s="49"/>
-      <c r="D65" s="49"/>
-      <c r="E65" s="49"/>
-      <c r="F65" s="49"/>
-      <c r="G65" s="50"/>
-      <c r="H65" s="50"/>
-      <c r="M65" s="23"/>
-      <c r="N65" s="23"/>
-      <c r="O65" s="23"/>
-      <c r="P65" s="23"/>
-    </row>
-    <row r="66" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C66" s="49"/>
-      <c r="D66" s="49"/>
-      <c r="E66" s="49"/>
-      <c r="F66" s="49"/>
-      <c r="G66" s="50"/>
-      <c r="H66" s="50"/>
-      <c r="M66" s="23"/>
-      <c r="N66" s="23"/>
-      <c r="O66" s="23"/>
-      <c r="P66" s="23"/>
-    </row>
-    <row r="67" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C67" s="49"/>
-      <c r="D67" s="49"/>
-      <c r="E67" s="49"/>
-      <c r="F67" s="49"/>
-      <c r="G67" s="50"/>
-      <c r="H67" s="50"/>
-      <c r="M67" s="23"/>
-      <c r="N67" s="23"/>
-      <c r="O67" s="23"/>
-      <c r="P67" s="23"/>
-    </row>
-    <row r="68" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C68" s="49"/>
-      <c r="D68" s="49"/>
-      <c r="E68" s="49"/>
-      <c r="F68" s="49"/>
-      <c r="G68" s="50"/>
-      <c r="H68" s="50"/>
-      <c r="M68" s="23"/>
-      <c r="N68" s="23"/>
-      <c r="O68" s="23"/>
-      <c r="P68" s="23"/>
-    </row>
-    <row r="69" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C69" s="49"/>
-      <c r="D69" s="49"/>
-      <c r="E69" s="49"/>
-      <c r="F69" s="49"/>
-      <c r="G69" s="49"/>
-      <c r="H69" s="49"/>
-    </row>
-    <row r="70" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C70" s="49"/>
-      <c r="D70" s="49"/>
-      <c r="E70" s="49"/>
-      <c r="F70" s="49"/>
-      <c r="G70" s="49"/>
-      <c r="H70" s="49"/>
-    </row>
-    <row r="71" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C71" s="49"/>
-      <c r="D71" s="49"/>
-      <c r="E71" s="49"/>
-      <c r="F71" s="49"/>
-      <c r="G71" s="49"/>
-      <c r="H71" s="49"/>
-    </row>
-    <row r="72" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C72" s="49"/>
-      <c r="D72" s="49"/>
-      <c r="E72" s="49"/>
-      <c r="F72" s="49"/>
-      <c r="G72" s="50"/>
-      <c r="H72" s="50"/>
-    </row>
-    <row r="73" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C73" s="49"/>
-      <c r="D73" s="49"/>
-      <c r="E73" s="49"/>
-      <c r="F73" s="49"/>
-      <c r="G73" s="50"/>
-      <c r="H73" s="50"/>
-    </row>
-    <row r="74" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C74" s="49"/>
-      <c r="D74" s="49"/>
-      <c r="E74" s="49"/>
-      <c r="F74" s="49"/>
-      <c r="G74" s="50"/>
-      <c r="H74" s="50"/>
-    </row>
-    <row r="75" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C75" s="49"/>
-      <c r="D75" s="49"/>
-      <c r="E75" s="49"/>
-      <c r="F75" s="49"/>
-      <c r="G75" s="49"/>
-      <c r="H75" s="49"/>
-    </row>
-    <row r="76" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C76" s="49"/>
-      <c r="D76" s="49"/>
-      <c r="E76" s="49"/>
-      <c r="F76" s="49"/>
-      <c r="G76" s="49"/>
-      <c r="H76" s="49"/>
-    </row>
-    <row r="77" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C77" s="49"/>
-      <c r="D77" s="49"/>
-      <c r="E77" s="49"/>
-      <c r="F77" s="49"/>
-      <c r="G77" s="49"/>
-      <c r="H77" s="49"/>
-    </row>
-    <row r="78" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C78" s="49"/>
-      <c r="D78" s="49"/>
-      <c r="E78" s="49"/>
-      <c r="F78" s="49"/>
-      <c r="G78" s="49"/>
-      <c r="H78" s="49"/>
-    </row>
-    <row r="79" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C79" s="49"/>
-      <c r="D79" s="49"/>
-      <c r="E79" s="49"/>
-      <c r="F79" s="49"/>
-      <c r="G79" s="50"/>
-      <c r="H79" s="50"/>
-    </row>
-    <row r="80" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C80" s="49"/>
-      <c r="D80" s="49"/>
-      <c r="E80" s="49"/>
-      <c r="F80" s="49"/>
-      <c r="G80" s="49"/>
-      <c r="H80" s="49"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="42"/>
+      <c r="H64" s="42"/>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C65" s="42"/>
+      <c r="D65" s="42"/>
+      <c r="E65" s="42"/>
+      <c r="F65" s="42"/>
+      <c r="G65" s="43"/>
+      <c r="H65" s="43"/>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="43"/>
+      <c r="H66" s="43"/>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C67" s="42"/>
+      <c r="D67" s="42"/>
+      <c r="E67" s="42"/>
+      <c r="F67" s="42"/>
+      <c r="G67" s="43"/>
+      <c r="H67" s="43"/>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C68" s="42"/>
+      <c r="D68" s="42"/>
+      <c r="E68" s="42"/>
+      <c r="F68" s="42"/>
+      <c r="G68" s="43"/>
+      <c r="H68" s="43"/>
+    </row>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C69" s="42"/>
+      <c r="D69" s="42"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="42"/>
+      <c r="G69" s="42"/>
+      <c r="H69" s="42"/>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C70" s="42"/>
+      <c r="D70" s="42"/>
+      <c r="E70" s="42"/>
+      <c r="F70" s="42"/>
+      <c r="G70" s="42"/>
+      <c r="H70" s="42"/>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C71" s="42"/>
+      <c r="D71" s="42"/>
+      <c r="E71" s="42"/>
+      <c r="F71" s="42"/>
+      <c r="G71" s="42"/>
+      <c r="H71" s="42"/>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C72" s="42"/>
+      <c r="D72" s="42"/>
+      <c r="E72" s="42"/>
+      <c r="F72" s="42"/>
+      <c r="G72" s="43"/>
+      <c r="H72" s="43"/>
+    </row>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C73" s="42"/>
+      <c r="D73" s="42"/>
+      <c r="E73" s="42"/>
+      <c r="F73" s="42"/>
+      <c r="G73" s="43"/>
+      <c r="H73" s="43"/>
+    </row>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C74" s="42"/>
+      <c r="D74" s="42"/>
+      <c r="E74" s="42"/>
+      <c r="F74" s="42"/>
+      <c r="G74" s="43"/>
+      <c r="H74" s="43"/>
+    </row>
+    <row r="75" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C75" s="42"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="42"/>
+      <c r="F75" s="42"/>
+      <c r="G75" s="42"/>
+      <c r="H75" s="42"/>
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C76" s="42"/>
+      <c r="D76" s="42"/>
+      <c r="E76" s="42"/>
+      <c r="F76" s="42"/>
+      <c r="G76" s="42"/>
+      <c r="H76" s="42"/>
+    </row>
+    <row r="77" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C77" s="42"/>
+      <c r="D77" s="42"/>
+      <c r="E77" s="42"/>
+      <c r="F77" s="42"/>
+      <c r="G77" s="42"/>
+      <c r="H77" s="42"/>
+    </row>
+    <row r="78" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C78" s="42"/>
+      <c r="D78" s="42"/>
+      <c r="E78" s="42"/>
+      <c r="F78" s="42"/>
+      <c r="G78" s="42"/>
+      <c r="H78" s="42"/>
+    </row>
+    <row r="79" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C79" s="42"/>
+      <c r="D79" s="42"/>
+      <c r="E79" s="42"/>
+      <c r="F79" s="42"/>
+      <c r="G79" s="43"/>
+      <c r="H79" s="43"/>
+    </row>
+    <row r="80" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C80" s="42"/>
+      <c r="D80" s="42"/>
+      <c r="E80" s="42"/>
+      <c r="F80" s="42"/>
+      <c r="G80" s="42"/>
+      <c r="H80" s="42"/>
     </row>
     <row r="81" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C81" s="49"/>
-      <c r="D81" s="49"/>
-      <c r="E81" s="49"/>
-      <c r="F81" s="49"/>
-      <c r="G81" s="49"/>
-      <c r="H81" s="49"/>
+      <c r="C81" s="42"/>
+      <c r="D81" s="42"/>
+      <c r="E81" s="42"/>
+      <c r="F81" s="42"/>
+      <c r="G81" s="42"/>
+      <c r="H81" s="42"/>
     </row>
     <row r="82" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C82" s="49"/>
-      <c r="D82" s="49"/>
-      <c r="E82" s="49"/>
-      <c r="F82" s="49"/>
-      <c r="G82" s="49"/>
-      <c r="H82" s="49"/>
+      <c r="C82" s="42"/>
+      <c r="D82" s="42"/>
+      <c r="E82" s="42"/>
+      <c r="F82" s="42"/>
+      <c r="G82" s="42"/>
+      <c r="H82" s="42"/>
     </row>
     <row r="83" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C83" s="49"/>
-      <c r="D83" s="49"/>
-      <c r="E83" s="49"/>
-      <c r="F83" s="49"/>
-      <c r="G83" s="50"/>
-      <c r="H83" s="50"/>
+      <c r="C83" s="42"/>
+      <c r="D83" s="42"/>
+      <c r="E83" s="42"/>
+      <c r="F83" s="42"/>
+      <c r="G83" s="43"/>
+      <c r="H83" s="43"/>
     </row>
     <row r="84" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C84" s="49"/>
-      <c r="D84" s="49"/>
-      <c r="E84" s="49"/>
-      <c r="F84" s="49"/>
-      <c r="G84" s="50"/>
-      <c r="H84" s="50"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="42"/>
+      <c r="F84" s="42"/>
+      <c r="G84" s="43"/>
+      <c r="H84" s="43"/>
     </row>
     <row r="85" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C85" s="49"/>
-      <c r="D85" s="49"/>
-      <c r="E85" s="49"/>
-      <c r="F85" s="49"/>
-      <c r="G85" s="49"/>
-      <c r="H85" s="49"/>
+      <c r="C85" s="42"/>
+      <c r="D85" s="42"/>
+      <c r="E85" s="42"/>
+      <c r="F85" s="42"/>
+      <c r="G85" s="42"/>
+      <c r="H85" s="42"/>
     </row>
     <row r="86" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C86" s="49"/>
-      <c r="D86" s="49"/>
-      <c r="E86" s="49"/>
-      <c r="F86" s="49"/>
-      <c r="G86" s="49"/>
-      <c r="H86" s="49"/>
+      <c r="C86" s="42"/>
+      <c r="D86" s="42"/>
+      <c r="E86" s="42"/>
+      <c r="F86" s="42"/>
+      <c r="G86" s="42"/>
+      <c r="H86" s="42"/>
     </row>
     <row r="87" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C87" s="49"/>
-      <c r="D87" s="49"/>
-      <c r="E87" s="49"/>
-      <c r="F87" s="49"/>
-      <c r="G87" s="49"/>
-      <c r="H87" s="49"/>
+      <c r="C87" s="42"/>
+      <c r="D87" s="42"/>
+      <c r="E87" s="42"/>
+      <c r="F87" s="42"/>
+      <c r="G87" s="42"/>
+      <c r="H87" s="42"/>
     </row>
     <row r="88" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C88" s="49"/>
-      <c r="D88" s="49"/>
-      <c r="E88" s="49"/>
-      <c r="F88" s="49"/>
-      <c r="G88" s="49"/>
-      <c r="H88" s="49"/>
+      <c r="C88" s="42"/>
+      <c r="D88" s="42"/>
+      <c r="E88" s="42"/>
+      <c r="F88" s="42"/>
+      <c r="G88" s="42"/>
+      <c r="H88" s="42"/>
     </row>
     <row r="89" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C89" s="49"/>
-      <c r="D89" s="49"/>
-      <c r="E89" s="49"/>
-      <c r="F89" s="49"/>
-      <c r="G89" s="49"/>
-      <c r="H89" s="49"/>
+      <c r="C89" s="42"/>
+      <c r="D89" s="42"/>
+      <c r="E89" s="42"/>
+      <c r="F89" s="42"/>
+      <c r="G89" s="42"/>
+      <c r="H89" s="42"/>
     </row>
     <row r="90" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C90" s="49"/>
-      <c r="D90" s="49"/>
-      <c r="E90" s="49"/>
-      <c r="F90" s="49"/>
-      <c r="G90" s="50"/>
-      <c r="H90" s="50"/>
+      <c r="C90" s="42"/>
+      <c r="D90" s="42"/>
+      <c r="E90" s="42"/>
+      <c r="F90" s="42"/>
+      <c r="G90" s="43"/>
+      <c r="H90" s="43"/>
     </row>
     <row r="91" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C91" s="49"/>
-      <c r="D91" s="49"/>
-      <c r="E91" s="49"/>
-      <c r="F91" s="49"/>
-      <c r="G91" s="50"/>
-      <c r="H91" s="50"/>
+      <c r="C91" s="42"/>
+      <c r="D91" s="42"/>
+      <c r="E91" s="42"/>
+      <c r="F91" s="42"/>
+      <c r="G91" s="43"/>
+      <c r="H91" s="43"/>
     </row>
     <row r="92" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C92" s="49"/>
-      <c r="D92" s="49"/>
-      <c r="E92" s="49"/>
-      <c r="F92" s="49"/>
-      <c r="G92" s="49"/>
-      <c r="H92" s="49"/>
+      <c r="C92" s="42"/>
+      <c r="D92" s="42"/>
+      <c r="E92" s="42"/>
+      <c r="F92" s="42"/>
+      <c r="G92" s="42"/>
+      <c r="H92" s="42"/>
     </row>
     <row r="93" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C93" s="49"/>
-      <c r="D93" s="49"/>
-      <c r="E93" s="49"/>
-      <c r="F93" s="49"/>
-      <c r="G93" s="50"/>
-      <c r="H93" s="50"/>
+      <c r="C93" s="42"/>
+      <c r="D93" s="42"/>
+      <c r="E93" s="42"/>
+      <c r="F93" s="42"/>
+      <c r="G93" s="43"/>
+      <c r="H93" s="43"/>
     </row>
     <row r="94" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C94" s="49"/>
-      <c r="D94" s="49"/>
-      <c r="E94" s="49"/>
-      <c r="F94" s="49"/>
-      <c r="G94" s="50"/>
-      <c r="H94" s="50"/>
+      <c r="C94" s="42"/>
+      <c r="D94" s="42"/>
+      <c r="E94" s="42"/>
+      <c r="F94" s="42"/>
+      <c r="G94" s="43"/>
+      <c r="H94" s="43"/>
     </row>
     <row r="95" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C95" s="49"/>
-      <c r="D95" s="49"/>
-      <c r="E95" s="49"/>
-      <c r="F95" s="49"/>
-      <c r="G95" s="49"/>
-      <c r="H95" s="49"/>
+      <c r="C95" s="42"/>
+      <c r="D95" s="42"/>
+      <c r="E95" s="42"/>
+      <c r="F95" s="42"/>
+      <c r="G95" s="42"/>
+      <c r="H95" s="42"/>
     </row>
     <row r="96" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C96" s="49"/>
-      <c r="D96" s="49"/>
-      <c r="E96" s="49"/>
-      <c r="F96" s="49"/>
-      <c r="G96" s="49"/>
-      <c r="H96" s="49"/>
+      <c r="C96" s="42"/>
+      <c r="D96" s="42"/>
+      <c r="E96" s="42"/>
+      <c r="F96" s="42"/>
+      <c r="G96" s="42"/>
+      <c r="H96" s="42"/>
     </row>
     <row r="97" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C97" s="49"/>
-      <c r="D97" s="49"/>
-      <c r="E97" s="49"/>
-      <c r="F97" s="49"/>
-      <c r="G97" s="49"/>
-      <c r="H97" s="49"/>
+      <c r="C97" s="42"/>
+      <c r="D97" s="42"/>
+      <c r="E97" s="42"/>
+      <c r="F97" s="42"/>
+      <c r="G97" s="42"/>
+      <c r="H97" s="42"/>
     </row>
     <row r="98" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C98" s="49"/>
-      <c r="D98" s="49"/>
-      <c r="E98" s="49"/>
-      <c r="F98" s="49"/>
-      <c r="G98" s="49"/>
-      <c r="H98" s="49"/>
+      <c r="C98" s="42"/>
+      <c r="D98" s="42"/>
+      <c r="E98" s="42"/>
+      <c r="F98" s="42"/>
+      <c r="G98" s="42"/>
+      <c r="H98" s="42"/>
     </row>
     <row r="99" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C99" s="49"/>
-      <c r="D99" s="49"/>
-      <c r="E99" s="49"/>
-      <c r="F99" s="49"/>
-      <c r="G99" s="49"/>
-      <c r="H99" s="49"/>
+      <c r="C99" s="42"/>
+      <c r="D99" s="42"/>
+      <c r="E99" s="42"/>
+      <c r="F99" s="42"/>
+      <c r="G99" s="42"/>
+      <c r="H99" s="42"/>
     </row>
     <row r="100" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C100" s="49"/>
-      <c r="D100" s="49"/>
-      <c r="E100" s="49"/>
-      <c r="F100" s="49"/>
-      <c r="G100" s="49"/>
-      <c r="H100" s="49"/>
+      <c r="C100" s="42"/>
+      <c r="D100" s="42"/>
+      <c r="E100" s="42"/>
+      <c r="F100" s="42"/>
+      <c r="G100" s="42"/>
+      <c r="H100" s="42"/>
     </row>
     <row r="101" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C101" s="49"/>
-      <c r="D101" s="49"/>
-      <c r="E101" s="49"/>
-      <c r="F101" s="49"/>
-      <c r="G101" s="49"/>
-      <c r="H101" s="49"/>
+      <c r="C101" s="42"/>
+      <c r="D101" s="42"/>
+      <c r="E101" s="42"/>
+      <c r="F101" s="42"/>
+      <c r="G101" s="42"/>
+      <c r="H101" s="42"/>
     </row>
     <row r="102" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C102" s="49"/>
-      <c r="D102" s="49"/>
-      <c r="E102" s="49"/>
-      <c r="F102" s="49"/>
-      <c r="G102" s="50"/>
-      <c r="H102" s="50"/>
+      <c r="C102" s="42"/>
+      <c r="D102" s="42"/>
+      <c r="E102" s="42"/>
+      <c r="F102" s="42"/>
+      <c r="G102" s="43"/>
+      <c r="H102" s="43"/>
     </row>
     <row r="103" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C103" s="49"/>
-      <c r="D103" s="49"/>
-      <c r="E103" s="49"/>
-      <c r="F103" s="49"/>
-      <c r="G103" s="50"/>
-      <c r="H103" s="50"/>
+      <c r="C103" s="42"/>
+      <c r="D103" s="42"/>
+      <c r="E103" s="42"/>
+      <c r="F103" s="42"/>
+      <c r="G103" s="43"/>
+      <c r="H103" s="43"/>
     </row>
     <row r="104" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C104" s="49"/>
-      <c r="D104" s="49"/>
-      <c r="E104" s="49"/>
-      <c r="F104" s="49"/>
-      <c r="G104" s="50"/>
-      <c r="H104" s="50"/>
+      <c r="C104" s="42"/>
+      <c r="D104" s="42"/>
+      <c r="E104" s="42"/>
+      <c r="F104" s="42"/>
+      <c r="G104" s="43"/>
+      <c r="H104" s="43"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F29:F30 F41">
-    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:F47">
-    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F50:F52">
-    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F55:F59">
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:F43">
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:F49">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F53:F54">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60:F61">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F31:F38 M31:M36">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  <conditionalFormatting sqref="F31:F38">
+    <cfRule type="duplicateValues" dxfId="23" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F31:F38 M38:M45">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  <conditionalFormatting sqref="F31:F38">
+    <cfRule type="duplicateValues" dxfId="22" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F31:F38 M47:M50">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  <conditionalFormatting sqref="F31:F38">
+    <cfRule type="duplicateValues" dxfId="21" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F31:F38 M52:M55">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  <conditionalFormatting sqref="F31:F38">
+    <cfRule type="duplicateValues" dxfId="20" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39 M37">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  <conditionalFormatting sqref="F39">
+    <cfRule type="duplicateValues" dxfId="19" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39 M46">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="F39">
+    <cfRule type="duplicateValues" dxfId="18" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39 M51">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="F39">
+    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39 M56">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="F39">
+    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>